<commit_message>
Updated amperage for rasp. pi in Part Count.xlsx
</commit_message>
<xml_diff>
--- a/Part Count.xlsx
+++ b/Part Count.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
       </c>
       <c r="C18">
         <f>SUM(C12:C16)</f>
-        <v>8.5800000000000018</v>
+        <v>8.3800000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>